<commit_message>
modif code + sper + specs
</commit_message>
<xml_diff>
--- a/01 - TRAVAIL/00 - Suivi/SPER.xlsx
+++ b/01 - TRAVAIL/00 - Suivi/SPER.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\Études\POLYTECH\5A\PRI\01 - TRAVAIL\00 - Suivi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF59C9B-7728-4FE0-8328-045636AB0149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E494C70-BF6D-4462-9C34-BAEFCF4C8227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6542,22 +6542,22 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.125</c:v>
+                  <c:v>0.10416666666666667</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.13541666666666666</c:v>
+                  <c:v>0.30927835051546393</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.13541666666666666</c:v>
+                  <c:v>0.30927835051546393</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.13541666666666666</c:v>
+                  <c:v>0.30927835051546393</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.13541666666666666</c:v>
+                  <c:v>0.30927835051546393</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.13541666666666666</c:v>
+                  <c:v>0.30927835051546393</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6951,19 +6951,19 @@
                   <c:v>350</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>385</c:v>
+                  <c:v>1050</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>385</c:v>
+                  <c:v>1050</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>385</c:v>
+                  <c:v>1050</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>385</c:v>
+                  <c:v>1050</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>385</c:v>
+                  <c:v>1050</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7576,7 +7576,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Synthèse!$F$4:$F$9</c:f>
+              <c:f>Synthèse!$E$4:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -7584,19 +7584,19 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9445,7 +9445,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>828675</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>6745</xdr:rowOff>
@@ -9487,7 +9487,7 @@
       <xdr:rowOff>16271</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>790575</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>14287</xdr:rowOff>
@@ -10078,7 +10078,7 @@
   <dimension ref="B2:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.46484375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10087,8 +10087,8 @@
     <col min="2" max="2" width="9.73046875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.3984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.06640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.86328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.9296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.9296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.86328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.59765625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.53125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.3984375" bestFit="1" customWidth="1"/>
@@ -10104,10 +10104,10 @@
         <v>58</v>
       </c>
       <c r="E3" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="66" t="s">
         <v>59</v>
-      </c>
-      <c r="F3" s="66" t="s">
-        <v>60</v>
       </c>
       <c r="G3" s="66" t="s">
         <v>61</v>
@@ -10132,12 +10132,12 @@
         <v>96</v>
       </c>
       <c r="E4" s="63">
+        <f>-Septembre[[#Totals],[Écart de Charge (h)]]</f>
+        <v>2</v>
+      </c>
+      <c r="F4" s="63">
         <f>Septembre[[#Totals],[Temps Passé Cumul (h)]]</f>
         <v>10</v>
-      </c>
-      <c r="F4" s="63">
-        <f>-Septembre[[#Totals],[Écart de Charge (h)]]</f>
-        <v>2</v>
       </c>
       <c r="G4" s="63">
         <f>Septembre[[#Totals],[Coût Initial (€)]]</f>
@@ -10148,8 +10148,8 @@
         <v>350</v>
       </c>
       <c r="I4" s="64">
-        <f>IFERROR((E4+F4)/D4,0)</f>
-        <v>0.125</v>
+        <f>IFERROR(F4/D4,0)</f>
+        <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.45">
@@ -10162,15 +10162,15 @@
       </c>
       <c r="D5" s="2">
         <f>Octobre[[#Totals],[Charge Révisée (h)]]</f>
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E5" s="2">
+        <f>-Octobre[[#Totals],[Écart de Charge (h)]]</f>
+        <v>3</v>
+      </c>
+      <c r="F5" s="2">
         <f>Octobre[[#Totals],[Temps Passé Cumul (h)]]</f>
-        <v>11</v>
-      </c>
-      <c r="F5" s="2">
-        <f>-Octobre[[#Totals],[Écart de Charge (h)]]</f>
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="G5" s="2">
         <f>Octobre[[#Totals],[Coût Initial (€)]]</f>
@@ -10178,11 +10178,11 @@
       </c>
       <c r="H5" s="54">
         <f>Octobre[[#Totals],[Coût Réel (€)]]</f>
-        <v>385</v>
+        <v>1050</v>
       </c>
       <c r="I5" s="57">
-        <f t="shared" ref="I5:I9" si="0">IFERROR((E5+F5)/D5,0)</f>
-        <v>0.13541666666666666</v>
+        <f t="shared" ref="I5:I9" si="0">IFERROR(F5/D5,0)</f>
+        <v>0.30927835051546393</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.45">
@@ -10195,15 +10195,15 @@
       </c>
       <c r="D6" s="2">
         <f>Novembre[[#Totals],[Charge Révisée (h)]]</f>
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E6" s="2">
+        <f>-Novembre[[#Totals],[Écart de Charge (h)]]</f>
+        <v>3</v>
+      </c>
+      <c r="F6" s="2">
         <f>Novembre[[#Totals],[Temps Passé Cumul (h)]]</f>
-        <v>11</v>
-      </c>
-      <c r="F6" s="2">
-        <f>-Novembre[[#Totals],[Écart de Charge (h)]]</f>
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="G6" s="2">
         <f>Novembre[[#Totals],[Coût Initial (€)]]</f>
@@ -10211,11 +10211,11 @@
       </c>
       <c r="H6" s="54">
         <f>Novembre[[#Totals],[Coût Réel (€)]]</f>
-        <v>385</v>
+        <v>1050</v>
       </c>
       <c r="I6" s="57">
         <f t="shared" si="0"/>
-        <v>0.13541666666666666</v>
+        <v>0.30927835051546393</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.45">
@@ -10228,15 +10228,15 @@
       </c>
       <c r="D7" s="2">
         <f>Décembre[[#Totals],[Charge Révisée (h)]]</f>
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E7" s="2">
+        <f>-Décembre[[#Totals],[Écart de Charge (h)]]</f>
+        <v>3</v>
+      </c>
+      <c r="F7" s="2">
         <f>Décembre[[#Totals],[Temps Passé Cumul (h)]]</f>
-        <v>11</v>
-      </c>
-      <c r="F7" s="2">
-        <f>-Décembre[[#Totals],[Écart de Charge (h)]]</f>
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="G7" s="2">
         <f>Décembre[[#Totals],[Coût Initial (€)]]</f>
@@ -10244,11 +10244,11 @@
       </c>
       <c r="H7" s="54">
         <f>Décembre[[#Totals],[Coût Réel (€)]]</f>
-        <v>385</v>
+        <v>1050</v>
       </c>
       <c r="I7" s="57">
         <f t="shared" si="0"/>
-        <v>0.13541666666666666</v>
+        <v>0.30927835051546393</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.45">
@@ -10261,15 +10261,15 @@
       </c>
       <c r="D8" s="2">
         <f>Janvier[[#Totals],[Charge Révisée (h)]]</f>
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E8" s="2">
+        <f>-Janvier[[#Totals],[Écart de Charge (h)]]</f>
+        <v>3</v>
+      </c>
+      <c r="F8" s="2">
         <f>Janvier[[#Totals],[Temps Passé Cumul (h)]]</f>
-        <v>11</v>
-      </c>
-      <c r="F8" s="2">
-        <f>-Janvier[[#Totals],[Écart de Charge (h)]]</f>
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="G8" s="2">
         <f>Janvier[[#Totals],[Coût Initial (€)]]</f>
@@ -10277,11 +10277,11 @@
       </c>
       <c r="H8" s="54">
         <f>Janvier[[#Totals],[Coût Réel (€)]]</f>
-        <v>385</v>
+        <v>1050</v>
       </c>
       <c r="I8" s="57">
         <f t="shared" si="0"/>
-        <v>0.13541666666666666</v>
+        <v>0.30927835051546393</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -10294,15 +10294,15 @@
       </c>
       <c r="D9" s="53">
         <f>Février[[#Totals],[Charge Révisée (h)]]</f>
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E9" s="53">
+        <f>-Février[[#Totals],[Écart de Charge (h)]]</f>
+        <v>3</v>
+      </c>
+      <c r="F9" s="53">
         <f>Février[[#Totals],[Temps Passé Cumul (h)]]</f>
-        <v>11</v>
-      </c>
-      <c r="F9" s="53">
-        <f>-Février[[#Totals],[Écart de Charge (h)]]</f>
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="G9" s="53">
         <f>Février[[#Totals],[Coût Initial (€)]]</f>
@@ -10310,11 +10310,11 @@
       </c>
       <c r="H9" s="55">
         <f>Février[[#Totals],[Coût Réel (€)]]</f>
-        <v>385</v>
+        <v>1050</v>
       </c>
       <c r="I9" s="58">
         <f t="shared" si="0"/>
-        <v>0.13541666666666666</v>
+        <v>0.30927835051546393</v>
       </c>
     </row>
   </sheetData>
@@ -11581,11 +11581,11 @@
         <v>5</v>
       </c>
       <c r="E2" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="22">
         <f>Octobre[[#This Row],[Temps Passé Période (h)]]+Septembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G2" s="22">
         <f>MAX(Octobre[[#This Row],[Charge Initiale (h)]]-Octobre[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
@@ -11593,11 +11593,11 @@
       </c>
       <c r="H2" s="22">
         <f>Octobre[[#This Row],[Temps Passé Cumul (h)]]+Octobre[[#This Row],[Reste à Passer (h)]]</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I2" s="22">
         <f>Octobre[[#This Row],[Charge Initiale (h)]]-Octobre[[#This Row],[Charge Révisée (h)]]</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J2" s="22" t="str">
         <f>IF(Octobre[[#This Row],[Qui]]="Chef de projet","35",IF(Octobre[[#This Row],[Qui]]="Ingénieur Electronique","32",IF(Octobre[[#This Row],[Qui]]="Ingénieur qualité","36",IF(Octobre[[#This Row],[Qui]]="Ingénieur Développement",30,IF(Octobre[[#This Row],[Qui]]="Ingénieur Mécanique",34,"")))))</f>
@@ -11609,11 +11609,11 @@
       </c>
       <c r="L2" s="22">
         <f>Octobre[[#This Row],[Charge Révisée (h)]]*Octobre[[#This Row],[Prix de Revient Unitaire (€)]]</f>
-        <v>210</v>
+        <v>245</v>
       </c>
       <c r="M2" s="22">
         <f>Octobre[[#This Row],[Prix de Revient Unitaire (€)]]*Octobre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>210</v>
+        <v>245</v>
       </c>
       <c r="N2" s="23" t="s">
         <v>28</v>
@@ -11631,15 +11631,15 @@
         <v>5</v>
       </c>
       <c r="E3" s="22">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F3" s="22">
         <f>Octobre[[#This Row],[Temps Passé Période (h)]]+Septembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G3" s="22">
         <f>MAX(Octobre[[#This Row],[Charge Initiale (h)]]-Octobre[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H3" s="22">
         <f>Octobre[[#This Row],[Temps Passé Cumul (h)]]+Octobre[[#This Row],[Reste à Passer (h)]]</f>
@@ -11663,10 +11663,10 @@
       </c>
       <c r="M3" s="22">
         <f>Octobre[[#This Row],[Prix de Revient Unitaire (€)]]*Octobre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="N3" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.45">
@@ -11731,15 +11731,15 @@
         <v>2</v>
       </c>
       <c r="E5" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5" s="22">
         <f>Octobre[[#This Row],[Temps Passé Période (h)]]+Septembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G5" s="22">
         <f>MAX(Octobre[[#This Row],[Charge Initiale (h)]]-Octobre[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H5" s="22">
         <f>Octobre[[#This Row],[Temps Passé Cumul (h)]]+Octobre[[#This Row],[Reste à Passer (h)]]</f>
@@ -11763,10 +11763,10 @@
       </c>
       <c r="M5" s="22">
         <f>Octobre[[#This Row],[Prix de Revient Unitaire (€)]]*Octobre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="N5" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.45">
@@ -11783,15 +11783,15 @@
         <v>8</v>
       </c>
       <c r="E6" s="4">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F6" s="4">
         <f>Octobre[[#This Row],[Temps Passé Période (h)]]+Septembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G6" s="4">
         <f>MAX(Octobre[[#This Row],[Charge Initiale (h)]]-Octobre[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="H6" s="4">
         <f>Octobre[[#This Row],[Temps Passé Cumul (h)]]+Octobre[[#This Row],[Reste à Passer (h)]]</f>
@@ -11815,10 +11815,10 @@
       </c>
       <c r="M6" s="4">
         <f>Octobre[[#This Row],[Prix de Revient Unitaire (€)]]*Octobre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>35</v>
+        <v>280</v>
       </c>
       <c r="N6" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.45">
@@ -11833,15 +11833,15 @@
         <v>3</v>
       </c>
       <c r="E7" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F7" s="4">
         <f>Octobre[[#This Row],[Temps Passé Période (h)]]+Septembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G7" s="4">
         <f>MAX(Octobre[[#This Row],[Charge Initiale (h)]]-Octobre[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H7" s="4">
         <f>Octobre[[#This Row],[Temps Passé Cumul (h)]]+Octobre[[#This Row],[Reste à Passer (h)]]</f>
@@ -11865,10 +11865,10 @@
       </c>
       <c r="M7" s="4">
         <f>Octobre[[#This Row],[Prix de Revient Unitaire (€)]]*Octobre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.45">
@@ -11883,15 +11883,15 @@
         <v>3</v>
       </c>
       <c r="E8" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F8" s="4">
         <f>Octobre[[#This Row],[Temps Passé Période (h)]]+Septembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G8" s="4">
         <f>MAX(Octobre[[#This Row],[Charge Initiale (h)]]-Octobre[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H8" s="4">
         <f>Octobre[[#This Row],[Temps Passé Cumul (h)]]+Octobre[[#This Row],[Reste à Passer (h)]]</f>
@@ -11915,10 +11915,10 @@
       </c>
       <c r="M8" s="4">
         <f>Octobre[[#This Row],[Prix de Revient Unitaire (€)]]*Octobre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="N8" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.45">
@@ -12547,23 +12547,23 @@
       </c>
       <c r="E21" s="15">
         <f>SUBTOTAL(109,Octobre[Temps Passé Période (h)])</f>
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F21" s="15">
         <f>SUBTOTAL(109,Octobre[Temps Passé Cumul (h)])</f>
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G21" s="15">
         <f>SUBTOTAL(109,Octobre[Reste à Passer (h)])</f>
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="H21" s="15">
         <f>SUBTOTAL(109,Octobre[Charge Révisée (h)])</f>
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I21" s="15">
         <f>SUBTOTAL(109,Octobre[Écart de Charge (h)])</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J21" s="15">
         <f>SUBTOTAL(109,Octobre[Prix de Revient Unitaire (€)])</f>
@@ -12575,11 +12575,11 @@
       </c>
       <c r="L21" s="16">
         <f>SUBTOTAL(109,Octobre[Coût Révisé (€)])</f>
-        <v>3360</v>
+        <v>3395</v>
       </c>
       <c r="M21" s="15">
         <f>SUBTOTAL(109,Octobre[Coût Réel (€)])</f>
-        <v>385</v>
+        <v>1050</v>
       </c>
       <c r="N21" s="17"/>
     </row>
@@ -12639,7 +12639,7 @@
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A13:A14"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N20" xr:uid="{3CF902A2-AA41-422F-9FCE-C4D9D5F29CCF}">
       <formula1>$M$24:$M$25</formula1>
     </dataValidation>
@@ -12750,7 +12750,7 @@
       </c>
       <c r="F2" s="22">
         <f>Novembre[[#This Row],[Temps Passé Période (h)]]+Octobre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G2" s="22">
         <f>MAX(Novembre[[#This Row],[Charge Initiale (h)]]-Novembre[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
@@ -12758,11 +12758,11 @@
       </c>
       <c r="H2" s="22">
         <f>Novembre[[#This Row],[Temps Passé Cumul (h)]]+Novembre[[#This Row],[Reste à Passer (h)]]</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I2" s="22">
         <f>Novembre[[#This Row],[Charge Initiale (h)]]-Novembre[[#This Row],[Charge Révisée (h)]]</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J2" s="22" t="str">
         <f>IF(Novembre[[#This Row],[Qui]]="Chef de projet","35",IF(Novembre[[#This Row],[Qui]]="Ingénieur Electronique","32",IF(Novembre[[#This Row],[Qui]]="Ingénieur qualité","36",IF(Novembre[[#This Row],[Qui]]="Ingénieur Développement",30,IF(Novembre[[#This Row],[Qui]]="Ingénieur Mécanique",34,"")))))</f>
@@ -12774,11 +12774,11 @@
       </c>
       <c r="L2" s="22">
         <f>Novembre[[#This Row],[Charge Révisée (h)]]*Novembre[[#This Row],[Prix de Revient Unitaire (€)]]</f>
-        <v>210</v>
+        <v>245</v>
       </c>
       <c r="M2" s="22">
         <f>Novembre[[#This Row],[Prix de Revient Unitaire (€)]]*Novembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>210</v>
+        <v>245</v>
       </c>
       <c r="N2" s="23" t="s">
         <v>28</v>
@@ -12800,11 +12800,11 @@
       </c>
       <c r="F3" s="22">
         <f>Novembre[[#This Row],[Temps Passé Période (h)]]+Octobre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G3" s="22">
         <f>MAX(Novembre[[#This Row],[Charge Initiale (h)]]-Novembre[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H3" s="22">
         <f>Novembre[[#This Row],[Temps Passé Cumul (h)]]+Novembre[[#This Row],[Reste à Passer (h)]]</f>
@@ -12828,10 +12828,10 @@
       </c>
       <c r="M3" s="22">
         <f>Novembre[[#This Row],[Prix de Revient Unitaire (€)]]*Novembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="N3" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.45">
@@ -12900,11 +12900,11 @@
       </c>
       <c r="F5" s="22">
         <f>Novembre[[#This Row],[Temps Passé Période (h)]]+Octobre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G5" s="22">
         <f>MAX(Novembre[[#This Row],[Charge Initiale (h)]]-Novembre[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H5" s="22">
         <f>Novembre[[#This Row],[Temps Passé Cumul (h)]]+Novembre[[#This Row],[Reste à Passer (h)]]</f>
@@ -12928,10 +12928,10 @@
       </c>
       <c r="M5" s="22">
         <f>Novembre[[#This Row],[Prix de Revient Unitaire (€)]]*Novembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="N5" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.45">
@@ -12952,11 +12952,11 @@
       </c>
       <c r="F6" s="4">
         <f>Novembre[[#This Row],[Temps Passé Période (h)]]+Octobre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G6" s="4">
         <f>MAX(Novembre[[#This Row],[Charge Initiale (h)]]-Novembre[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="H6" s="4">
         <f>Novembre[[#This Row],[Temps Passé Cumul (h)]]+Novembre[[#This Row],[Reste à Passer (h)]]</f>
@@ -12980,10 +12980,10 @@
       </c>
       <c r="M6" s="4">
         <f>Novembre[[#This Row],[Prix de Revient Unitaire (€)]]*Novembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>35</v>
+        <v>280</v>
       </c>
       <c r="N6" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.45">
@@ -13002,11 +13002,11 @@
       </c>
       <c r="F7" s="4">
         <f>Novembre[[#This Row],[Temps Passé Période (h)]]+Octobre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G7" s="4">
         <f>MAX(Novembre[[#This Row],[Charge Initiale (h)]]-Novembre[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H7" s="4">
         <f>Novembre[[#This Row],[Temps Passé Cumul (h)]]+Novembre[[#This Row],[Reste à Passer (h)]]</f>
@@ -13030,10 +13030,10 @@
       </c>
       <c r="M7" s="4">
         <f>Novembre[[#This Row],[Prix de Revient Unitaire (€)]]*Novembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.45">
@@ -13052,11 +13052,11 @@
       </c>
       <c r="F8" s="4">
         <f>Novembre[[#This Row],[Temps Passé Période (h)]]+Octobre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G8" s="4">
         <f>MAX(Novembre[[#This Row],[Charge Initiale (h)]]-Novembre[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H8" s="4">
         <f>Novembre[[#This Row],[Temps Passé Cumul (h)]]+Novembre[[#This Row],[Reste à Passer (h)]]</f>
@@ -13080,10 +13080,10 @@
       </c>
       <c r="M8" s="4">
         <f>Novembre[[#This Row],[Prix de Revient Unitaire (€)]]*Novembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="N8" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.45">
@@ -13716,19 +13716,19 @@
       </c>
       <c r="F21" s="15">
         <f>SUBTOTAL(109,Novembre[Temps Passé Cumul (h)])</f>
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G21" s="15">
         <f>SUBTOTAL(109,Novembre[Reste à Passer (h)])</f>
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="H21" s="15">
         <f>SUBTOTAL(109,Novembre[Charge Révisée (h)])</f>
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I21" s="15">
         <f>SUBTOTAL(109,Novembre[Écart de Charge (h)])</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J21" s="15">
         <f>SUBTOTAL(109,Novembre[Prix de Revient Unitaire (€)])</f>
@@ -13740,11 +13740,11 @@
       </c>
       <c r="L21" s="16">
         <f>SUBTOTAL(109,Novembre[Coût Révisé (€)])</f>
-        <v>3360</v>
+        <v>3395</v>
       </c>
       <c r="M21" s="15">
         <f>SUBTOTAL(109,Novembre[Coût Réel (€)])</f>
-        <v>385</v>
+        <v>1050</v>
       </c>
       <c r="N21" s="17"/>
     </row>
@@ -13804,7 +13804,7 @@
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A13:A14"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C20" xr:uid="{85D63007-F628-426F-8751-2AE10528A7C2}">
       <formula1>$B$24:$B$24</formula1>
     </dataValidation>
@@ -13915,7 +13915,7 @@
       </c>
       <c r="F2" s="22">
         <f>Décembre[[#This Row],[Temps Passé Période (h)]]+Novembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G2" s="22">
         <f>MAX(Décembre[[#This Row],[Charge Initiale (h)]]-Décembre[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
@@ -13923,11 +13923,11 @@
       </c>
       <c r="H2" s="22">
         <f>Décembre[[#This Row],[Temps Passé Cumul (h)]]+Décembre[[#This Row],[Reste à Passer (h)]]</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I2" s="22">
         <f>Décembre[[#This Row],[Charge Initiale (h)]]-Décembre[[#This Row],[Charge Révisée (h)]]</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J2" s="22" t="str">
         <f>IF(Décembre[[#This Row],[Qui]]="Chef de projet","35",IF(Décembre[[#This Row],[Qui]]="Ingénieur Electronique","32",IF(Décembre[[#This Row],[Qui]]="Ingénieur qualité","36",IF(Décembre[[#This Row],[Qui]]="Ingénieur Développement",30,IF(Décembre[[#This Row],[Qui]]="Ingénieur Mécanique",34,"")))))</f>
@@ -13939,11 +13939,11 @@
       </c>
       <c r="L2" s="22">
         <f>Décembre[[#This Row],[Charge Révisée (h)]]*Décembre[[#This Row],[Prix de Revient Unitaire (€)]]</f>
-        <v>210</v>
+        <v>245</v>
       </c>
       <c r="M2" s="22">
         <f>Décembre[[#This Row],[Prix de Revient Unitaire (€)]]*Décembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>210</v>
+        <v>245</v>
       </c>
       <c r="N2" s="23" t="s">
         <v>28</v>
@@ -13965,11 +13965,11 @@
       </c>
       <c r="F3" s="22">
         <f>Décembre[[#This Row],[Temps Passé Période (h)]]+Novembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G3" s="22">
         <f>MAX(Décembre[[#This Row],[Charge Initiale (h)]]-Décembre[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H3" s="22">
         <f>Décembre[[#This Row],[Temps Passé Cumul (h)]]+Décembre[[#This Row],[Reste à Passer (h)]]</f>
@@ -13993,7 +13993,7 @@
       </c>
       <c r="M3" s="22">
         <f>Décembre[[#This Row],[Prix de Revient Unitaire (€)]]*Décembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="N3" s="23" t="s">
         <v>29</v>
@@ -14065,11 +14065,11 @@
       </c>
       <c r="F5" s="22">
         <f>Décembre[[#This Row],[Temps Passé Période (h)]]+Novembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G5" s="22">
         <f>MAX(Décembre[[#This Row],[Charge Initiale (h)]]-Décembre[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H5" s="22">
         <f>Décembre[[#This Row],[Temps Passé Cumul (h)]]+Décembre[[#This Row],[Reste à Passer (h)]]</f>
@@ -14093,7 +14093,7 @@
       </c>
       <c r="M5" s="22">
         <f>Décembre[[#This Row],[Prix de Revient Unitaire (€)]]*Décembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="N5" s="23" t="s">
         <v>29</v>
@@ -14117,11 +14117,11 @@
       </c>
       <c r="F6" s="4">
         <f>Décembre[[#This Row],[Temps Passé Période (h)]]+Novembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G6" s="4">
         <f>MAX(Décembre[[#This Row],[Charge Initiale (h)]]-Décembre[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="H6" s="4">
         <f>Décembre[[#This Row],[Temps Passé Cumul (h)]]+Décembre[[#This Row],[Reste à Passer (h)]]</f>
@@ -14145,7 +14145,7 @@
       </c>
       <c r="M6" s="4">
         <f>Décembre[[#This Row],[Prix de Revient Unitaire (€)]]*Décembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>35</v>
+        <v>280</v>
       </c>
       <c r="N6" s="12" t="s">
         <v>29</v>
@@ -14167,11 +14167,11 @@
       </c>
       <c r="F7" s="4">
         <f>Décembre[[#This Row],[Temps Passé Période (h)]]+Novembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G7" s="4">
         <f>MAX(Décembre[[#This Row],[Charge Initiale (h)]]-Décembre[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H7" s="4">
         <f>Décembre[[#This Row],[Temps Passé Cumul (h)]]+Décembre[[#This Row],[Reste à Passer (h)]]</f>
@@ -14195,7 +14195,7 @@
       </c>
       <c r="M7" s="4">
         <f>Décembre[[#This Row],[Prix de Revient Unitaire (€)]]*Décembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="N7" s="12" t="s">
         <v>29</v>
@@ -14217,11 +14217,11 @@
       </c>
       <c r="F8" s="4">
         <f>Décembre[[#This Row],[Temps Passé Période (h)]]+Novembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G8" s="4">
         <f>MAX(Décembre[[#This Row],[Charge Initiale (h)]]-Décembre[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H8" s="4">
         <f>Décembre[[#This Row],[Temps Passé Cumul (h)]]+Décembre[[#This Row],[Reste à Passer (h)]]</f>
@@ -14245,7 +14245,7 @@
       </c>
       <c r="M8" s="4">
         <f>Décembre[[#This Row],[Prix de Revient Unitaire (€)]]*Décembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="N8" s="12" t="s">
         <v>29</v>
@@ -14881,19 +14881,19 @@
       </c>
       <c r="F21" s="15">
         <f>SUBTOTAL(109,Décembre[Temps Passé Cumul (h)])</f>
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G21" s="15">
         <f>SUBTOTAL(109,Décembre[Reste à Passer (h)])</f>
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="H21" s="15">
         <f>SUBTOTAL(109,Décembre[Charge Révisée (h)])</f>
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I21" s="15">
         <f>SUBTOTAL(109,Décembre[Écart de Charge (h)])</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J21" s="15">
         <f>SUBTOTAL(109,Décembre[Prix de Revient Unitaire (€)])</f>
@@ -14905,11 +14905,11 @@
       </c>
       <c r="L21" s="16">
         <f>SUBTOTAL(109,Décembre[Coût Révisé (€)])</f>
-        <v>3360</v>
+        <v>3395</v>
       </c>
       <c r="M21" s="15">
         <f>SUBTOTAL(109,Décembre[Coût Réel (€)])</f>
-        <v>385</v>
+        <v>1050</v>
       </c>
       <c r="N21" s="17"/>
     </row>
@@ -15080,7 +15080,7 @@
       </c>
       <c r="F2" s="22">
         <f>Janvier[[#This Row],[Temps Passé Période (h)]]+Décembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G2" s="22">
         <f>MAX(Janvier[[#This Row],[Charge Initiale (h)]]-Janvier[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
@@ -15088,11 +15088,11 @@
       </c>
       <c r="H2" s="22">
         <f>Janvier[[#This Row],[Temps Passé Cumul (h)]]+Janvier[[#This Row],[Reste à Passer (h)]]</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I2" s="22">
         <f>Janvier[[#This Row],[Charge Initiale (h)]]-Janvier[[#This Row],[Charge Révisée (h)]]</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J2" s="22" t="str">
         <f>IF(Janvier[[#This Row],[Qui]]="Chef de projet","35",IF(Janvier[[#This Row],[Qui]]="Ingénieur Electronique","32",IF(Janvier[[#This Row],[Qui]]="Ingénieur qualité","36",IF(Janvier[[#This Row],[Qui]]="Ingénieur Développement",30,IF(Janvier[[#This Row],[Qui]]="Ingénieur Mécanique",34,"")))))</f>
@@ -15104,11 +15104,11 @@
       </c>
       <c r="L2" s="22">
         <f>Janvier[[#This Row],[Charge Révisée (h)]]*Janvier[[#This Row],[Prix de Revient Unitaire (€)]]</f>
-        <v>210</v>
+        <v>245</v>
       </c>
       <c r="M2" s="22">
         <f>Janvier[[#This Row],[Prix de Revient Unitaire (€)]]*Janvier[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>210</v>
+        <v>245</v>
       </c>
       <c r="N2" s="23" t="s">
         <v>28</v>
@@ -15130,11 +15130,11 @@
       </c>
       <c r="F3" s="22">
         <f>Janvier[[#This Row],[Temps Passé Période (h)]]+Décembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G3" s="22">
         <f>MAX(Janvier[[#This Row],[Charge Initiale (h)]]-Janvier[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H3" s="22">
         <f>Janvier[[#This Row],[Temps Passé Cumul (h)]]+Janvier[[#This Row],[Reste à Passer (h)]]</f>
@@ -15158,7 +15158,7 @@
       </c>
       <c r="M3" s="22">
         <f>Janvier[[#This Row],[Prix de Revient Unitaire (€)]]*Janvier[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="N3" s="23" t="s">
         <v>29</v>
@@ -15230,11 +15230,11 @@
       </c>
       <c r="F5" s="22">
         <f>Janvier[[#This Row],[Temps Passé Période (h)]]+Décembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G5" s="22">
         <f>MAX(Janvier[[#This Row],[Charge Initiale (h)]]-Janvier[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H5" s="22">
         <f>Janvier[[#This Row],[Temps Passé Cumul (h)]]+Janvier[[#This Row],[Reste à Passer (h)]]</f>
@@ -15258,7 +15258,7 @@
       </c>
       <c r="M5" s="22">
         <f>Janvier[[#This Row],[Prix de Revient Unitaire (€)]]*Janvier[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="N5" s="23" t="s">
         <v>29</v>
@@ -15282,11 +15282,11 @@
       </c>
       <c r="F6" s="4">
         <f>Janvier[[#This Row],[Temps Passé Période (h)]]+Décembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G6" s="4">
         <f>MAX(Janvier[[#This Row],[Charge Initiale (h)]]-Janvier[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="H6" s="4">
         <f>Janvier[[#This Row],[Temps Passé Cumul (h)]]+Janvier[[#This Row],[Reste à Passer (h)]]</f>
@@ -15310,7 +15310,7 @@
       </c>
       <c r="M6" s="4">
         <f>Janvier[[#This Row],[Prix de Revient Unitaire (€)]]*Janvier[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>35</v>
+        <v>280</v>
       </c>
       <c r="N6" s="12" t="s">
         <v>29</v>
@@ -15332,11 +15332,11 @@
       </c>
       <c r="F7" s="4">
         <f>Janvier[[#This Row],[Temps Passé Période (h)]]+Décembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G7" s="4">
         <f>MAX(Janvier[[#This Row],[Charge Initiale (h)]]-Janvier[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H7" s="4">
         <f>Janvier[[#This Row],[Temps Passé Cumul (h)]]+Janvier[[#This Row],[Reste à Passer (h)]]</f>
@@ -15360,7 +15360,7 @@
       </c>
       <c r="M7" s="4">
         <f>Janvier[[#This Row],[Prix de Revient Unitaire (€)]]*Janvier[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="N7" s="12" t="s">
         <v>29</v>
@@ -15382,11 +15382,11 @@
       </c>
       <c r="F8" s="4">
         <f>Janvier[[#This Row],[Temps Passé Période (h)]]+Décembre[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G8" s="4">
         <f>MAX(Janvier[[#This Row],[Charge Initiale (h)]]-Janvier[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H8" s="4">
         <f>Janvier[[#This Row],[Temps Passé Cumul (h)]]+Janvier[[#This Row],[Reste à Passer (h)]]</f>
@@ -15410,7 +15410,7 @@
       </c>
       <c r="M8" s="4">
         <f>Janvier[[#This Row],[Prix de Revient Unitaire (€)]]*Janvier[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="N8" s="12" t="s">
         <v>29</v>
@@ -16046,19 +16046,19 @@
       </c>
       <c r="F21" s="15">
         <f>SUBTOTAL(109,Janvier[Temps Passé Cumul (h)])</f>
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G21" s="15">
         <f>SUBTOTAL(109,Janvier[Reste à Passer (h)])</f>
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="H21" s="15">
         <f>SUBTOTAL(109,Janvier[Charge Révisée (h)])</f>
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I21" s="15">
         <f>SUBTOTAL(109,Janvier[Écart de Charge (h)])</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J21" s="15">
         <f>SUBTOTAL(109,Janvier[Prix de Revient Unitaire (€)])</f>
@@ -16070,11 +16070,11 @@
       </c>
       <c r="L21" s="16">
         <f>SUBTOTAL(109,Janvier[Coût Révisé (€)])</f>
-        <v>3360</v>
+        <v>3395</v>
       </c>
       <c r="M21" s="15">
         <f>SUBTOTAL(109,Janvier[Coût Réel (€)])</f>
-        <v>385</v>
+        <v>1050</v>
       </c>
       <c r="N21" s="17"/>
     </row>
@@ -16245,7 +16245,7 @@
       </c>
       <c r="F2" s="22">
         <f>Février[[#This Row],[Temps Passé Période (h)]]+Janvier[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G2" s="22">
         <f>MAX(Février[[#This Row],[Charge Initiale (h)]]-Février[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
@@ -16253,11 +16253,11 @@
       </c>
       <c r="H2" s="22">
         <f>Février[[#This Row],[Temps Passé Cumul (h)]]+Février[[#This Row],[Reste à Passer (h)]]</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I2" s="22">
         <f>Février[[#This Row],[Charge Initiale (h)]]-Février[[#This Row],[Charge Révisée (h)]]</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="J2" s="22" t="str">
         <f>IF(Février[[#This Row],[Qui]]="Chef de projet","35",IF(Février[[#This Row],[Qui]]="Ingénieur Electronique","32",IF(Février[[#This Row],[Qui]]="Ingénieur qualité","36",IF(Février[[#This Row],[Qui]]="Ingénieur Développement",30,IF(Février[[#This Row],[Qui]]="Ingénieur Mécanique",34,"")))))</f>
@@ -16269,11 +16269,11 @@
       </c>
       <c r="L2" s="22">
         <f>Février[[#This Row],[Charge Révisée (h)]]*Février[[#This Row],[Prix de Revient Unitaire (€)]]</f>
-        <v>210</v>
+        <v>245</v>
       </c>
       <c r="M2" s="22">
         <f>Février[[#This Row],[Prix de Revient Unitaire (€)]]*Février[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>210</v>
+        <v>245</v>
       </c>
       <c r="N2" s="23" t="s">
         <v>28</v>
@@ -16295,11 +16295,11 @@
       </c>
       <c r="F3" s="22">
         <f>Février[[#This Row],[Temps Passé Période (h)]]+Janvier[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G3" s="22">
         <f>MAX(Février[[#This Row],[Charge Initiale (h)]]-Février[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H3" s="22">
         <f>Février[[#This Row],[Temps Passé Cumul (h)]]+Février[[#This Row],[Reste à Passer (h)]]</f>
@@ -16323,7 +16323,7 @@
       </c>
       <c r="M3" s="22">
         <f>Février[[#This Row],[Prix de Revient Unitaire (€)]]*Février[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="N3" s="23" t="s">
         <v>29</v>
@@ -16395,11 +16395,11 @@
       </c>
       <c r="F5" s="22">
         <f>Février[[#This Row],[Temps Passé Période (h)]]+Janvier[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G5" s="22">
         <f>MAX(Février[[#This Row],[Charge Initiale (h)]]-Février[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H5" s="22">
         <f>Février[[#This Row],[Temps Passé Cumul (h)]]+Février[[#This Row],[Reste à Passer (h)]]</f>
@@ -16423,7 +16423,7 @@
       </c>
       <c r="M5" s="22">
         <f>Février[[#This Row],[Prix de Revient Unitaire (€)]]*Février[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="N5" s="23" t="s">
         <v>29</v>
@@ -16447,11 +16447,11 @@
       </c>
       <c r="F6" s="4">
         <f>Février[[#This Row],[Temps Passé Période (h)]]+Janvier[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G6" s="4">
         <f>MAX(Février[[#This Row],[Charge Initiale (h)]]-Février[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="H6" s="4">
         <f>Février[[#This Row],[Temps Passé Cumul (h)]]+Février[[#This Row],[Reste à Passer (h)]]</f>
@@ -16475,7 +16475,7 @@
       </c>
       <c r="M6" s="4">
         <f>Février[[#This Row],[Prix de Revient Unitaire (€)]]*Février[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>35</v>
+        <v>280</v>
       </c>
       <c r="N6" s="12" t="s">
         <v>29</v>
@@ -16497,11 +16497,11 @@
       </c>
       <c r="F7" s="4">
         <f>Février[[#This Row],[Temps Passé Période (h)]]+Janvier[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G7" s="4">
         <f>MAX(Février[[#This Row],[Charge Initiale (h)]]-Février[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H7" s="4">
         <f>Février[[#This Row],[Temps Passé Cumul (h)]]+Février[[#This Row],[Reste à Passer (h)]]</f>
@@ -16525,7 +16525,7 @@
       </c>
       <c r="M7" s="4">
         <f>Février[[#This Row],[Prix de Revient Unitaire (€)]]*Février[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="N7" s="12" t="s">
         <v>29</v>
@@ -16547,11 +16547,11 @@
       </c>
       <c r="F8" s="4">
         <f>Février[[#This Row],[Temps Passé Période (h)]]+Janvier[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G8" s="4">
         <f>MAX(Février[[#This Row],[Charge Initiale (h)]]-Février[[#This Row],[Temps Passé Cumul (h)]], 0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H8" s="4">
         <f>Février[[#This Row],[Temps Passé Cumul (h)]]+Février[[#This Row],[Reste à Passer (h)]]</f>
@@ -16575,7 +16575,7 @@
       </c>
       <c r="M8" s="4">
         <f>Février[[#This Row],[Prix de Revient Unitaire (€)]]*Février[[#This Row],[Temps Passé Cumul (h)]]</f>
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="N8" s="12" t="s">
         <v>29</v>
@@ -17211,19 +17211,19 @@
       </c>
       <c r="F21" s="15">
         <f>SUBTOTAL(109,Février[Temps Passé Cumul (h)])</f>
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G21" s="15">
         <f>SUBTOTAL(109,Février[Reste à Passer (h)])</f>
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="H21" s="15">
         <f>SUBTOTAL(109,Février[Charge Révisée (h)])</f>
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I21" s="15">
         <f>SUBTOTAL(109,Février[Écart de Charge (h)])</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J21" s="15">
         <f>SUBTOTAL(109,Février[Prix de Revient Unitaire (€)])</f>
@@ -17235,11 +17235,11 @@
       </c>
       <c r="L21" s="16">
         <f>SUBTOTAL(109,Février[Coût Révisé (€)])</f>
-        <v>3360</v>
+        <v>3395</v>
       </c>
       <c r="M21" s="15">
         <f>SUBTOTAL(109,Février[Coût Réel (€)])</f>
-        <v>385</v>
+        <v>1050</v>
       </c>
       <c r="N21" s="17"/>
     </row>
@@ -17320,26 +17320,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="1ee72ef8-afb7-4cab-8045-23d1f296c8e3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f3823e97-3c8f-42af-9aa3-4a85adc1b986">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CF9263497045A640A8CB558901A6A6C8" ma:contentTypeVersion="11" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="74a64c617853225d9915ce5c2407eb7f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f3823e97-3c8f-42af-9aa3-4a85adc1b986" xmlns:ns3="1ee72ef8-afb7-4cab-8045-23d1f296c8e3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2245405c225123f82bf2fff4f792a1eb" ns2:_="" ns3:_="">
     <xsd:import namespace="f3823e97-3c8f-42af-9aa3-4a85adc1b986"/>
@@ -17534,32 +17514,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3B8A56E-0482-4C34-B391-4275AF43D713}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="1ee72ef8-afb7-4cab-8045-23d1f296c8e3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f3823e97-3c8f-42af-9aa3-4a85adc1b986">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DD8CA4D-88CF-4FAD-9219-4EDEC6099C12}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="1ee72ef8-afb7-4cab-8045-23d1f296c8e3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="f3823e97-3c8f-42af-9aa3-4a85adc1b986"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B8A2DB-F0C8-46F4-AC39-BA8B306E6417}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17576,4 +17551,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DD8CA4D-88CF-4FAD-9219-4EDEC6099C12}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="1ee72ef8-afb7-4cab-8045-23d1f296c8e3"/>
+    <ds:schemaRef ds:uri="f3823e97-3c8f-42af-9aa3-4a85adc1b986"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3B8A56E-0482-4C34-B391-4275AF43D713}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>